<commit_message>
updates done 4:00pm 03-02-2026
</commit_message>
<xml_diff>
--- a/Excel Output/Hotel Details.xlsx
+++ b/Excel Output/Hotel Details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>S.No</t>
   </si>
@@ -29,28 +29,22 @@
     <t>Holiday Inn NAIROBI TWO RIVERS MALL by IHG</t>
   </si>
   <si>
-    <t>₹ 19,978</t>
+    <t>₹ 19,986</t>
   </si>
   <si>
-    <t>₹ 127,861</t>
+    <t>N/A</t>
   </si>
   <si>
     <t>JW Marriott Hotel Nairobi</t>
   </si>
   <si>
-    <t>₹ 203,323</t>
-  </si>
-  <si>
-    <t>₹ 1,283,575</t>
+    <t>₹ 203,399</t>
   </si>
   <si>
     <t>Yaya Hotel &amp; Apartments</t>
   </si>
   <si>
-    <t>₹ 19,625</t>
-  </si>
-  <si>
-    <t>₹ 96,160</t>
+    <t>₹ 19,632</t>
   </si>
 </sst>
 </file>
@@ -140,7 +134,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -148,13 +142,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="C4" t="s" s="0">
-        <v>11</v>
-      </c>
       <c r="D4" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update of Guest Capacity method
</commit_message>
<xml_diff>
--- a/Excel Output/Hotel Details.xlsx
+++ b/Excel Output/Hotel Details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>S.No</t>
   </si>
@@ -32,7 +32,7 @@
     <t>₹ 19,986</t>
   </si>
   <si>
-    <t>N/A</t>
+    <t>₹ 127,909</t>
   </si>
   <si>
     <t>JW Marriott Hotel Nairobi</t>
@@ -41,10 +41,16 @@
     <t>₹ 203,399</t>
   </si>
   <si>
+    <t>₹ 1,284,055</t>
+  </si>
+  <si>
     <t>Yaya Hotel &amp; Apartments</t>
   </si>
   <si>
     <t>₹ 19,632</t>
+  </si>
+  <si>
+    <t>₹ 96,194</t>
   </si>
 </sst>
 </file>
@@ -134,7 +140,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -142,13 +148,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Date Validataions by Bhargav Raj
</commit_message>
<xml_diff>
--- a/Excel Output/Hotel Details.xlsx
+++ b/Excel Output/Hotel Details.xlsx
@@ -29,28 +29,28 @@
     <t>Holiday Inn NAIROBI TWO RIVERS MALL by IHG</t>
   </si>
   <si>
-    <t>₹ 21,887</t>
+    <t>₹ 20,452</t>
   </si>
   <si>
-    <t>₹ 140,077</t>
+    <t>₹ 130,890</t>
   </si>
   <si>
     <t>JW Marriott Hotel Nairobi</t>
   </si>
   <si>
-    <t>₹ 204,438</t>
+    <t>₹ 204,675</t>
   </si>
   <si>
-    <t>₹ 1,290,616</t>
+    <t>₹ 1,292,111</t>
   </si>
   <si>
     <t>Yaya Hotel &amp; Apartments</t>
   </si>
   <si>
-    <t>₹ 19,760</t>
+    <t>₹ 19,783</t>
   </si>
   <si>
-    <t>₹ 95,273</t>
+    <t>₹ 95,383</t>
   </si>
 </sst>
 </file>

</xml_diff>